<commit_message>
Translation Update (Fixed Items.xlsx)
</commit_message>
<xml_diff>
--- a/data/Enemies.xlsx
+++ b/data/Enemies.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128">
   <si>
     <t>テスト用雑魚</t>
   </si>
@@ -384,6 +384,9 @@
   </si>
   <si>
     <t>木材</t>
+  </si>
+  <si>
+    <t>Wood</t>
   </si>
   <si>
     <t>玄関扉</t>
@@ -1344,25 +1347,28 @@
       <c r="A114" t="s">
         <v>122</v>
       </c>
+      <c r="C114" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>